<commit_message>
progress ubah semua export menjadi method post
</commit_message>
<xml_diff>
--- a/public/reportdata/Debi-dev Summary Interval Report 11-02-2020 15.xlsx
+++ b/public/reportdata/Debi-dev Summary Interval Report 11-02-2020 15.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="108">
   <si>
     <t>Summary Interval - oct_telkomcare</t>
   </si>
@@ -25,13 +25,13 @@
     <t xml:space="preserve">Export Time </t>
   </si>
   <si>
-    <t>11-02-2020 15:08:04</t>
+    <t>11-02-2020 15:15:50</t>
   </si>
   <si>
     <t xml:space="preserve">Filter Date </t>
   </si>
   <si>
-    <t>2020-02-11</t>
+    <t>2020-01-01</t>
   </si>
   <si>
     <t xml:space="preserve">Export By </t>
@@ -73,7 +73,274 @@
     <t>Total Session (COF)</t>
   </si>
   <si>
-    <t>-</t>
+    <t>00:00:00-01:00:00</t>
+  </si>
+  <si>
+    <t>0:35:36</t>
+  </si>
+  <si>
+    <t>0:05:02</t>
+  </si>
+  <si>
+    <t>0:36:24</t>
+  </si>
+  <si>
+    <t>01:00:00-02:00:00</t>
+  </si>
+  <si>
+    <t>0:29:11</t>
+  </si>
+  <si>
+    <t>0:05:07</t>
+  </si>
+  <si>
+    <t>0:29:43</t>
+  </si>
+  <si>
+    <t>02:00:00-03:00:00</t>
+  </si>
+  <si>
+    <t>0:14:33</t>
+  </si>
+  <si>
+    <t>0:03:30</t>
+  </si>
+  <si>
+    <t>0:15:28</t>
+  </si>
+  <si>
+    <t>03:00:00-04:00:00</t>
+  </si>
+  <si>
+    <t>0:08:38</t>
+  </si>
+  <si>
+    <t>0:04:41</t>
+  </si>
+  <si>
+    <t>0:09:24</t>
+  </si>
+  <si>
+    <t>04:00:00-05:00:00</t>
+  </si>
+  <si>
+    <t>0:10:30</t>
+  </si>
+  <si>
+    <t>0:06:09</t>
+  </si>
+  <si>
+    <t>0:11:27</t>
+  </si>
+  <si>
+    <t>05:00:00-06:00:00</t>
+  </si>
+  <si>
+    <t>0:16:32</t>
+  </si>
+  <si>
+    <t>0:06:12</t>
+  </si>
+  <si>
+    <t>0:17:06</t>
+  </si>
+  <si>
+    <t>06:00:00-07:00:00</t>
+  </si>
+  <si>
+    <t>0:13:13</t>
+  </si>
+  <si>
+    <t>0:07:27</t>
+  </si>
+  <si>
+    <t>0:14:00</t>
+  </si>
+  <si>
+    <t>07:00:00-08:00:00</t>
+  </si>
+  <si>
+    <t>0:05:52</t>
+  </si>
+  <si>
+    <t>0:05:35</t>
+  </si>
+  <si>
+    <t>0:06:57</t>
+  </si>
+  <si>
+    <t>08:00:00-09:00:00</t>
+  </si>
+  <si>
+    <t>0:05:23</t>
+  </si>
+  <si>
+    <t>0:06:19</t>
+  </si>
+  <si>
+    <t>09:00:00-10:00:00</t>
+  </si>
+  <si>
+    <t>0:06:20</t>
+  </si>
+  <si>
+    <t>0:05:22</t>
+  </si>
+  <si>
+    <t>0:07:25</t>
+  </si>
+  <si>
+    <t>10:00:00-11:00:00</t>
+  </si>
+  <si>
+    <t>0:05:09</t>
+  </si>
+  <si>
+    <t>11:00:00-12:00:00</t>
+  </si>
+  <si>
+    <t>0:05:47</t>
+  </si>
+  <si>
+    <t>0:05:56</t>
+  </si>
+  <si>
+    <t>0:06:50</t>
+  </si>
+  <si>
+    <t>12:00:00-13:00:00</t>
+  </si>
+  <si>
+    <t>0:07:48</t>
+  </si>
+  <si>
+    <t>0:05:55</t>
+  </si>
+  <si>
+    <t>13:00:00-14:00:00</t>
+  </si>
+  <si>
+    <t>0:07:29</t>
+  </si>
+  <si>
+    <t>0:08:34</t>
+  </si>
+  <si>
+    <t>14:00:00-15:00:00</t>
+  </si>
+  <si>
+    <t>0:08:07</t>
+  </si>
+  <si>
+    <t>0:05:54</t>
+  </si>
+  <si>
+    <t>0:08:55</t>
+  </si>
+  <si>
+    <t>15:00:00-16:00:00</t>
+  </si>
+  <si>
+    <t>0:04:49</t>
+  </si>
+  <si>
+    <t>0:05:25</t>
+  </si>
+  <si>
+    <t>0:05:38</t>
+  </si>
+  <si>
+    <t>16:00:00-17:00:00</t>
+  </si>
+  <si>
+    <t>0:05:28</t>
+  </si>
+  <si>
+    <t>0:06:00</t>
+  </si>
+  <si>
+    <t>0:06:29</t>
+  </si>
+  <si>
+    <t>17:00:00-18:00:00</t>
+  </si>
+  <si>
+    <t>0:05:04</t>
+  </si>
+  <si>
+    <t>0:05:26</t>
+  </si>
+  <si>
+    <t>0:05:51</t>
+  </si>
+  <si>
+    <t>18:00:00-19:00:00</t>
+  </si>
+  <si>
+    <t>0:37:37</t>
+  </si>
+  <si>
+    <t>0:38:39</t>
+  </si>
+  <si>
+    <t>19:00:00-20:00:00</t>
+  </si>
+  <si>
+    <t>1:41:15</t>
+  </si>
+  <si>
+    <t>0:04:38</t>
+  </si>
+  <si>
+    <t>1:42:15</t>
+  </si>
+  <si>
+    <t>20:00:00-21:00:00</t>
+  </si>
+  <si>
+    <t>1:54:46</t>
+  </si>
+  <si>
+    <t>0:04:50</t>
+  </si>
+  <si>
+    <t>1:55:31</t>
+  </si>
+  <si>
+    <t>21:00:00-22:00:00</t>
+  </si>
+  <si>
+    <t>2:16:02</t>
+  </si>
+  <si>
+    <t>0:05:08</t>
+  </si>
+  <si>
+    <t>2:15:36</t>
+  </si>
+  <si>
+    <t>22:00:00-23:00:00</t>
+  </si>
+  <si>
+    <t>2:09:07</t>
+  </si>
+  <si>
+    <t>0:05:03</t>
+  </si>
+  <si>
+    <t>2:09:38</t>
+  </si>
+  <si>
+    <t>23:00:00-24:00:00</t>
+  </si>
+  <si>
+    <t>2:21:31</t>
+  </si>
+  <si>
+    <t>0:04:35</t>
+  </si>
+  <si>
+    <t>2:18:43</t>
   </si>
 </sst>
 </file>
@@ -481,10 +748,10 @@
   <cols>
     <col min="1" max="1" width="16.567383" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="23.422852" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="20.280762" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="21.137695" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="13.996582" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="4.570313" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="4.570313" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="9.283447" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="9.283447" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="12.854004" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="13.996582" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="23.422852" bestFit="true" customWidth="true" style="0"/>
@@ -556,361 +823,697 @@
       <c r="A5" s="4">
         <v>1</v>
       </c>
-      <c r="B5" s="4"/>
+      <c r="B5" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="C5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
+      <c r="D5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="4">
+        <v>51</v>
+      </c>
+      <c r="H5" s="4">
+        <v>38</v>
+      </c>
+      <c r="I5" s="4">
+        <v>334</v>
+      </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="4">
         <v>2</v>
       </c>
-      <c r="B6" s="4"/>
+      <c r="B6" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="C6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
+        <v>22</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="4">
+        <v>60</v>
+      </c>
+      <c r="H6" s="4">
+        <v>39</v>
+      </c>
+      <c r="I6" s="4">
+        <v>305</v>
+      </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="4">
         <v>3</v>
       </c>
-      <c r="B7" s="4"/>
+      <c r="B7" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="C7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
+        <v>26</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="4">
+        <v>19</v>
+      </c>
+      <c r="H7" s="4">
+        <v>14</v>
+      </c>
+      <c r="I7" s="4">
+        <v>132</v>
+      </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="4">
         <v>4</v>
       </c>
-      <c r="B8" s="4"/>
+      <c r="B8" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="C8" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="4">
+        <v>24</v>
+      </c>
+      <c r="H8" s="4">
+        <v>16</v>
+      </c>
+      <c r="I8" s="4">
+        <v>106</v>
+      </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="4">
         <v>5</v>
       </c>
-      <c r="B9" s="4"/>
+      <c r="B9" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="C9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
+        <v>34</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="4">
+        <v>4</v>
+      </c>
+      <c r="H9" s="4">
+        <v>4</v>
+      </c>
+      <c r="I9" s="4">
+        <v>94</v>
+      </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="4">
         <v>6</v>
       </c>
-      <c r="B10" s="4"/>
+      <c r="B10" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="C10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="4">
+        <v>20</v>
+      </c>
+      <c r="H10" s="4">
         <v>18</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
+      <c r="I10" s="4">
+        <v>152</v>
+      </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="4">
         <v>7</v>
       </c>
-      <c r="B11" s="4"/>
+      <c r="B11" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="C11" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
+        <v>42</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" s="4">
+        <v>30</v>
+      </c>
+      <c r="H11" s="4">
+        <v>28</v>
+      </c>
+      <c r="I11" s="4">
+        <v>199</v>
+      </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="4">
         <v>8</v>
       </c>
-      <c r="B12" s="4"/>
+      <c r="B12" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="C12" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
+        <v>46</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" s="4">
+        <v>55</v>
+      </c>
+      <c r="H12" s="4">
+        <v>45</v>
+      </c>
+      <c r="I12" s="4">
+        <v>374</v>
+      </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="4">
         <v>9</v>
       </c>
-      <c r="B13" s="4"/>
+      <c r="B13" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="C13" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
+        <v>50</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="4">
+        <v>77</v>
+      </c>
+      <c r="H13" s="4">
+        <v>63</v>
+      </c>
+      <c r="I13" s="4">
+        <v>596</v>
+      </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="4">
         <v>10</v>
       </c>
-      <c r="B14" s="4"/>
+      <c r="B14" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="C14" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
+        <v>53</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" s="4">
+        <v>62</v>
+      </c>
+      <c r="H14" s="4">
+        <v>51</v>
+      </c>
+      <c r="I14" s="4">
+        <v>627</v>
+      </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="4">
         <v>11</v>
       </c>
-      <c r="B15" s="4"/>
+      <c r="B15" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="C15" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
+        <v>57</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" s="4">
+        <v>146</v>
+      </c>
+      <c r="H15" s="4">
+        <v>112</v>
+      </c>
+      <c r="I15" s="4">
+        <v>751</v>
+      </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="4">
         <v>12</v>
       </c>
-      <c r="B16" s="4"/>
+      <c r="B16" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="C16" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
+        <v>59</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G16" s="4">
+        <v>135</v>
+      </c>
+      <c r="H16" s="4">
+        <v>96</v>
+      </c>
+      <c r="I16" s="4">
+        <v>871</v>
+      </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="4">
         <v>13</v>
       </c>
-      <c r="B17" s="4"/>
+      <c r="B17" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="C17" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
+        <v>63</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" s="4">
+        <v>94</v>
+      </c>
+      <c r="H17" s="4">
+        <v>67</v>
+      </c>
+      <c r="I17" s="4">
+        <v>743</v>
+      </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="4">
         <v>14</v>
       </c>
-      <c r="B18" s="4"/>
+      <c r="B18" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="C18" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
+        <v>66</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G18" s="4">
+        <v>94</v>
+      </c>
+      <c r="H18" s="4">
+        <v>71</v>
+      </c>
+      <c r="I18" s="4">
+        <v>680</v>
+      </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="4">
         <v>15</v>
       </c>
-      <c r="B19" s="4"/>
+      <c r="B19" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="C19" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
+        <v>69</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G19" s="4">
+        <v>109</v>
+      </c>
+      <c r="H19" s="4">
+        <v>78</v>
+      </c>
+      <c r="I19" s="4">
+        <v>713</v>
+      </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="4">
         <v>16</v>
       </c>
-      <c r="B20" s="4"/>
+      <c r="B20" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="C20" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
+        <v>73</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G20" s="4">
+        <v>90</v>
+      </c>
+      <c r="H20" s="4">
+        <v>57</v>
+      </c>
+      <c r="I20" s="4">
+        <v>683</v>
+      </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="4">
         <v>17</v>
       </c>
-      <c r="B21" s="4"/>
+      <c r="B21" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="C21" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
+        <v>77</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G21" s="4">
+        <v>142</v>
+      </c>
+      <c r="H21" s="4">
+        <v>94</v>
+      </c>
+      <c r="I21" s="4">
+        <v>713</v>
+      </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="4">
         <v>18</v>
       </c>
-      <c r="B22" s="4"/>
+      <c r="B22" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="C22" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
+        <v>81</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G22" s="4">
+        <v>123</v>
+      </c>
+      <c r="H22" s="4">
+        <v>76</v>
+      </c>
+      <c r="I22" s="4">
+        <v>845</v>
+      </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="4">
         <v>19</v>
       </c>
-      <c r="B23" s="4"/>
+      <c r="B23" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="C23" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
+        <v>85</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G23" s="4">
+        <v>465</v>
+      </c>
+      <c r="H23" s="4">
+        <v>290</v>
+      </c>
+      <c r="I23" s="4">
+        <v>1850</v>
+      </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="4">
         <v>20</v>
       </c>
-      <c r="B24" s="4"/>
+      <c r="B24" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="C24" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
+        <v>88</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G24" s="4">
+        <v>668</v>
+      </c>
+      <c r="H24" s="4">
+        <v>387</v>
+      </c>
+      <c r="I24" s="4">
+        <v>2579</v>
+      </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="4">
         <v>21</v>
       </c>
-      <c r="B25" s="4"/>
+      <c r="B25" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="C25" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
+        <v>92</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G25" s="4">
+        <v>373</v>
+      </c>
+      <c r="H25" s="4">
+        <v>237</v>
+      </c>
+      <c r="I25" s="4">
+        <v>1548</v>
+      </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="4">
         <v>22</v>
       </c>
-      <c r="B26" s="4"/>
+      <c r="B26" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="C26" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G26" s="4">
+        <v>360</v>
+      </c>
+      <c r="H26" s="4">
+        <v>239</v>
+      </c>
+      <c r="I26" s="4">
+        <v>1456</v>
+      </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="4">
         <v>23</v>
       </c>
-      <c r="B27" s="4"/>
+      <c r="B27" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="C27" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
+        <v>100</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="G27" s="4">
+        <v>208</v>
+      </c>
+      <c r="H27" s="4">
+        <v>150</v>
+      </c>
+      <c r="I27" s="4">
+        <v>1103</v>
+      </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="4">
         <v>24</v>
       </c>
-      <c r="B28" s="4"/>
+      <c r="B28" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="C28" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
+        <v>104</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="G28" s="4">
+        <v>130</v>
+      </c>
+      <c r="H28" s="4">
+        <v>49</v>
+      </c>
+      <c r="I28" s="4">
+        <v>609</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>